<commit_message>
Se Arreglaron cosas y se agregaron cuadros, Listo Integrales, falta hacer un par de Curvas
</commit_message>
<xml_diff>
--- a/Metodo Segundo Parcial/Metodos Diferenciacion.xlsx
+++ b/Metodo Segundo Parcial/Metodos Diferenciacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Analisis Numerico Git\Metodo Segundo Parcial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992EB5B0-B800-4A77-951E-B9DD91914787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF9C393-BEA3-4609-9348-6DFADA7EF202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metodo Derivacion Tres Puntos" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Metodo de Tres Puntos</t>
   </si>
@@ -86,6 +86,24 @@
   </si>
   <si>
     <t>La de la regresiva es la progresiva cambiandole los signos a los terminos y restando las H en vez de sumarlas</t>
+  </si>
+  <si>
+    <t>Progresiva: Usa puntos posteriores</t>
+  </si>
+  <si>
+    <t>Centrada: Usa puntos centrados</t>
+  </si>
+  <si>
+    <t>Regresiva: Usa puntos anteriores</t>
+  </si>
+  <si>
+    <t>Todo Explicado en la de Tres puntos</t>
+  </si>
+  <si>
+    <t>Progresiva:</t>
+  </si>
+  <si>
+    <t>Regresiva:</t>
   </si>
 </sst>
 </file>
@@ -262,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,7 +297,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -292,12 +310,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -322,11 +334,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -334,9 +346,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,6 +366,382 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{078DC2C5-DF8D-A040-FFB8-73779A9FC827}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11591925" y="628650"/>
+          <a:ext cx="4629150" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A2DD2B-DB8B-2270-9E01-9DDBB7211A83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11649075" y="1485900"/>
+          <a:ext cx="5153025" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06010BB8-3F6F-DDE5-6782-288BF9F2AE5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11620500" y="2181225"/>
+          <a:ext cx="4743450" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{980D1783-3881-28C1-DF90-84F7080DD96A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7715250" y="2009775"/>
+          <a:ext cx="3867150" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E67E191-1F40-C87D-F8E5-50BFCC290BB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7905750" y="2781300"/>
+          <a:ext cx="4257675" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B467FE93-4AF7-86B3-D08E-E7EBA02F1883}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7496175" y="3581400"/>
+          <a:ext cx="5153025" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -617,26 +1007,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:R15"/>
+  <dimension ref="B1:V15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-    </row>
-    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2" t="s">
@@ -649,12 +1039,15 @@
         <v>3</v>
       </c>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="V3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="39">
         <v>0.1</v>
       </c>
       <c r="D4" s="5">
@@ -665,28 +1058,28 @@
         <v>1</v>
       </c>
       <c r="F4" s="6">
-        <f>(-3*(E4)+4*(EXP(D4+C$4)*COS(D4+C$4))-(EXP(D4+2*C$4)*COS(D4+2*C$4)))/(2*C$4)</f>
+        <f>(-3*(E4)+4*(EXP(D5)*COS(D5))-(EXP(D6)*COS(D6)))/(2*C$4)</f>
         <v>1.0077132298087299</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="19" t="s">
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="21"/>
-    </row>
-    <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="19"/>
+    </row>
+    <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="5">
@@ -697,23 +1090,23 @@
         <v>1.0996496668294093</v>
       </c>
       <c r="F5" s="6">
-        <f>((EXP(D5+C$4)*COS(D5+C$4))-(EXP(D5-C$4)*COS(D5-C$4)))/(2*C$4)</f>
+        <f>((EXP(D6)*COS(D6))-(EXP(D4)*COS(D4)))/(2*C$4)</f>
         <v>0.98528010677945699</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="5">
@@ -724,14 +1117,14 @@
         <v>1.1970560213558914</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" ref="F6:F10" si="1">((EXP(D6+C$4)*COS(D6+C$4))-(EXP(D6-C$4)*COS(D6-C$4)))/(2*C$4)</f>
+        <f t="shared" ref="F6:F10" si="1">((EXP(D7)*COS(D7))-(EXP(D5)*COS(D5)))/(2*C$4)</f>
         <v>0.94959853607763267</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="5">
@@ -748,8 +1141,11 @@
       <c r="G7" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="5">
@@ -767,7 +1163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="5">
@@ -785,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="5">
@@ -803,7 +1199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="8">
@@ -814,87 +1210,91 @@
         <v>1.54020302543178</v>
       </c>
       <c r="F11" s="9">
-        <f>((EXP(D11-2*C$4)*COS(D11-2*C$4))-4*(EXP(D11-C$4)*COS(D11-C$4))+3*(E11))/(2*C$4)</f>
+        <f>((EXP(D9)*COS(D9))-4*(EXP(D10)*COS(D10))+3*(E11))/(2*C$4)</f>
         <v>0.2602997532218243</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="24"/>
-    </row>
-    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="I13" s="13" t="s">
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="22"/>
+      <c r="V11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="I13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="15"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="I14" s="28" t="s">
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="13"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="I14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="30"/>
-    </row>
-    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I15" s="16" t="s">
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="28"/>
+    </row>
+    <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="18"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFA29F8-CF0A-487F-9840-6D12D6554046}">
-  <dimension ref="B1:Q11"/>
+  <dimension ref="B1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="40"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="37"/>
+      <c r="E2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="41"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="2" t="s">
@@ -906,165 +1306,184 @@
       <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="31"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="39">
         <v>0.1</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="30">
         <v>0</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="31">
         <f>EXP(D4)*COS(D4)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="33">
-        <f>(-25*(EXP(D4)*COS(D4))+48*(EXP(D4+C$4)*COS(D4+C$4))-36*(EXP(D4+2*C$4)*COS(D4+2*C$4))+16*(EXP(D4+3*C$4)*COS(D4+3*C$4))-3*(EXP(D4+4*C$4)*COS(D4+4*C$4)))/(12*C$4)</f>
+      <c r="F4" s="31">
+        <f>(-25*(EXP(D4)*COS(D4))+48*(EXP(D5)*COS(D5))-36*(EXP(D6)*COS(D6))+16*(EXP(D7)*COS(D7))-3*(EXP(D8)*COS(D8)))/(12*C$4)</f>
         <v>1.0000771725466397</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="15"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="13"/>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="32">
+      <c r="D5" s="30">
         <v>0.1</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="31">
         <f t="shared" ref="E5:E11" si="0">EXP(D5)*COS(D5)</f>
         <v>1.0996496668294093</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="31">
         <f>((EXP(D5-2*C$4)*COS(D5-2*C$4))-8*(EXP(D5-C$4)*COS(D5-C$4))+8*(EXP(D5+C$4)*COS(D5+C$4))-(EXP(D5+2*C$4)*COS(D5+2*C$4)))/(12*C$4)</f>
         <v>0.9893298305394912</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="18"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="16"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D6" s="32">
+      <c r="D6" s="30">
         <v>0.2</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="31">
         <f t="shared" si="0"/>
         <v>1.1970560213558914</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="31">
         <f t="shared" ref="F6:F10" si="1">((EXP(D6-2*C$4)*COS(D6-2*C$4))-8*(EXP(D6-C$4)*COS(D6-C$4))+8*(EXP(D6+C$4)*COS(D6+C$4))-(EXP(D6+2*C$4)*COS(D6+2*C$4)))/(12*C$4)</f>
         <v>0.95441343236390852</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D7" s="32">
+    <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="30">
         <v>0.3</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="31">
         <f t="shared" si="0"/>
         <v>1.2895693740449359</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="31">
         <f t="shared" si="1"/>
         <v>0.89067064208190294</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D8" s="32">
+    <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="30">
         <v>0.4</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="31">
         <f t="shared" si="0"/>
         <v>1.3740615388875219</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="31">
         <f t="shared" si="1"/>
         <v>0.79312815092581057</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="32" t="s">
         <v>5</v>
       </c>
+      <c r="I8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D9" s="32">
+      <c r="D9" s="30">
         <v>0.5</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="31">
         <f t="shared" si="0"/>
         <v>1.4468890365841693</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="31">
         <f t="shared" si="1"/>
         <v>0.65645863498605694</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="32" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D10" s="32">
+      <c r="D10" s="30">
         <v>0.6</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="31">
         <f t="shared" si="0"/>
         <v>1.503859540558786</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="31">
         <f t="shared" si="1"/>
         <v>0.47502012738415433</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="32" t="s">
         <v>5</v>
       </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="35">
+      <c r="D11" s="33">
         <v>0.7</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="34">
         <f t="shared" si="0"/>
         <v>1.54020302543178</v>
       </c>
-      <c r="F11" s="36">
-        <f>(3*(EXP(D11-4*C$4)*COS(D11-4*C$4))-16*(EXP(D11-3*C$4)*COS(D11-3*C$4))+36*(EXP(D11-2*C$4)*COS(D11-2*C$4))-48*(EXP(D11-C$4)*COS(D11-C$4))+25*(EXP(D11)*COS(D11)))/(12*C$4)</f>
-        <v>0.24295542161442654</v>
-      </c>
-      <c r="G11" s="37" t="s">
+      <c r="F11" s="34">
+        <f>(3*(EXP(D7)*COS(D7))-16*(EXP(D8)*COS(D8))+36*(EXP(D9)*COS(D9))-48*(EXP(D10)*COS(D10))+25*(EXP(D11)*COS(D11)))/(12*C$4)</f>
+        <v>0.24295542161443248</v>
+      </c>
+      <c r="G11" s="35" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregados ejercicios de integral y diferenciacion
</commit_message>
<xml_diff>
--- a/Metodo Segundo Parcial/Metodos Diferenciacion.xlsx
+++ b/Metodo Segundo Parcial/Metodos Diferenciacion.xlsx
@@ -8,26 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Analisis Numerico Git\Metodo Segundo Parcial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2858A2FE-774D-498F-AAE9-7736A29FCFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ED1373-FE47-4E34-A0A3-9E6339871AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metodo Derivacion Tres Puntos" sheetId="1" r:id="rId1"/>
     <sheet name="Metodo Derivacion 5 Puntos" sheetId="2" r:id="rId2"/>
+    <sheet name="Ejercicio 2 TP" sheetId="3" r:id="rId3"/>
+    <sheet name="Ejercicio 2 CP" sheetId="4" r:id="rId4"/>
+    <sheet name="Ejercicio con metodos lineales" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="50">
   <si>
     <t>Metodo de Tres Puntos</t>
   </si>
@@ -115,12 +130,75 @@
   <si>
     <t xml:space="preserve">Este es el Optimo </t>
   </si>
+  <si>
+    <t>Metodo 5 puntos</t>
+  </si>
+  <si>
+    <t>Derivada real</t>
+  </si>
+  <si>
+    <t>F´calc</t>
+  </si>
+  <si>
+    <t>F´real</t>
+  </si>
+  <si>
+    <t>|E|</t>
+  </si>
+  <si>
+    <t>F´obtenida</t>
+  </si>
+  <si>
+    <t>Ejercicio 1</t>
+  </si>
+  <si>
+    <t>Metodo de Regresion Lineal Por Minimos Cuadrados</t>
+  </si>
+  <si>
+    <t>N:</t>
+  </si>
+  <si>
+    <t>Yi</t>
+  </si>
+  <si>
+    <t>(Xi)^2</t>
+  </si>
+  <si>
+    <t>Xi*Yi</t>
+  </si>
+  <si>
+    <t>//&lt;-Si requiero Ampliar el Rango Recordar llevarlo a uno Menos que la Sumatoria</t>
+  </si>
+  <si>
+    <t>A1:</t>
+  </si>
+  <si>
+    <t>A2:</t>
+  </si>
+  <si>
+    <t>//&lt;- Si requiero mas espacio Recordar cambiarle los 21 por la celda de la sumatoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//&lt;- Es la sumatoria, para no confundirse </t>
+  </si>
+  <si>
+    <t>Rta:</t>
+  </si>
+  <si>
+    <t>//&lt;- Si Requiero mas espacio llevar la sumatoria mas abajo y Recordar cambiarlo en  A1 y A0</t>
+  </si>
+  <si>
+    <t>Por metodo de progresion lineal tenemos que la funcion es: Y=1.8636+0.4545</t>
+  </si>
+  <si>
+    <t>SI ES LINEAL NO TIENE DERIVADA???</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +206,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,8 +246,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -286,11 +420,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +582,98 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,6 +689,889 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8738436383976596E-2"/>
+          <c:y val="0.28340027627500436"/>
+          <c:w val="0.82137085323350978"/>
+          <c:h val="0.53934452070618588"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ejercicio con metodos lineales'!$F$4:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ejercicio con metodos lineales'!$G$4:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF8E-469D-9375-515A22F8C117}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="706789024"/>
+        <c:axId val="706799584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="706789024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="706799584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="706799584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="706789024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,6 +1950,446 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>591003</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A8AF771-619D-8EE4-4DC1-CCAF0CCAD36C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6486525" y="552450"/>
+          <a:ext cx="3248478" cy="457264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>429078</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76264</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B94BAF7-60D3-4A8F-90A3-4608D752C84A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324600" y="1543050"/>
+          <a:ext cx="3248478" cy="457264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E71E31F-1F22-4B4F-BEB7-F30E320A535A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="600075"/>
+          <a:ext cx="2457450" cy="1057275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{953E6C35-F3A9-44AA-A53B-E001CD105ABD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="857250" y="2038350"/>
+          <a:ext cx="1933575" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>675704</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180865</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661559BE-5989-585D-0DAC-B9BD36118CE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7534275" y="2800350"/>
+          <a:ext cx="4571429" cy="876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A394417-FD58-CC71-DC59-3349F562DADF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>570929</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>199915</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B919CFB9-2CC7-C3F1-22D1-FDE73C1A76A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191500" y="5505450"/>
+          <a:ext cx="4571429" cy="876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Metodo Lineal"/>
+      <sheetName val="Metodo Exponencial"/>
+      <sheetName val="Metodo Potencia"/>
+      <sheetName val="Metodo Crecimiento"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="F4">
+            <v>1</v>
+          </cell>
+          <cell r="G4">
+            <v>0.5</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="F5">
+            <v>2</v>
+          </cell>
+          <cell r="G5">
+            <v>2.5</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="F6">
+            <v>3</v>
+          </cell>
+          <cell r="G6">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="F7">
+            <v>4</v>
+          </cell>
+          <cell r="G7">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="F8">
+            <v>5</v>
+          </cell>
+          <cell r="G8">
+            <v>3.5</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="F9">
+            <v>6</v>
+          </cell>
+          <cell r="G9">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="F10">
+            <v>7</v>
+          </cell>
+          <cell r="G10">
+            <v>5.5</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1019,8 +2655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFA29F8-CF0A-487F-9840-6D12D6554046}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,4 +3281,1765 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{205E532C-3E35-4A1A-A215-0E2412677F40}">
+  <dimension ref="B1:O18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <f>5*EXP(3*D4)*SIN(2*D4)</f>
+        <v>91.318635203333841</v>
+      </c>
+      <c r="F4" s="6">
+        <f>(-3*(E4)+4*(5*EXP(3*D5)*SIN(2*D5))-(5*EXP(3*D6)*SIN(2*D6)))/(2*C$4)</f>
+        <v>204.24858249400336</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" ref="E5:E14" si="0">5*EXP(3*D5)*SIN(2*D5)</f>
+        <v>109.60235532705481</v>
+      </c>
+      <c r="F5" s="6">
+        <f>((5*EXP(3*D6)*SIN(2*D6))-(5*EXP(3*D4)*SIN(2*D4)))/(2*C$4)</f>
+        <v>161.42581998041592</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>123.60379919941703</v>
+      </c>
+      <c r="F6" s="6">
+        <f>((5*EXP(3*D7)*SIN(2*D7))-(5*EXP(3*D5)*SIN(2*D5)))/(2*C$4)</f>
+        <v>88.663980495747907</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>127.33515142620439</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" ref="F7:F13" si="1">((5*EXP(3*D8)*SIN(2*D8))-(5*EXP(3*D6)*SIN(2*D6)))/(2*C$4)</f>
+        <v>-59.540729094989828</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>111.69565338041906</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="1"/>
+        <v>-319.0952997646279</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
+      <c r="K8" s="43">
+        <f>5*(EXP(3*J8)*3*SIN(2*J8)+COS(2*J8)*2*EXP(3*J8))</f>
+        <v>190.37057910064783</v>
+      </c>
+      <c r="M8" s="52">
+        <f>F4</f>
+        <v>204.24858249400336</v>
+      </c>
+      <c r="N8" s="52">
+        <f>K8</f>
+        <v>190.37057910064783</v>
+      </c>
+      <c r="O8" s="52">
+        <f>ABS(M8-N8)</f>
+        <v>13.878003393355527</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>63.516091473278813</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="1"/>
+        <v>-735.80493040668966</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K9" s="43">
+        <f t="shared" ref="K9:K18" si="2">5*(EXP(3*J9)*3*SIN(2*J9)+COS(2*J9)*2*EXP(3*J9))</f>
+        <v>169.24888301568495</v>
+      </c>
+      <c r="M9" s="52">
+        <f>F5</f>
+        <v>161.42581998041592</v>
+      </c>
+      <c r="N9" s="52">
+        <f>K9</f>
+        <v>169.24888301568495</v>
+      </c>
+      <c r="O9" s="52">
+        <f t="shared" ref="O9:O18" si="3">ABS(M9-N9)</f>
+        <v>7.8230630352690298</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>-35.465332700918879</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="1"/>
+        <v>-1365.4389310653848</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="K10" s="43">
+        <f t="shared" si="2"/>
+        <v>100.93831681151826</v>
+      </c>
+      <c r="M10" s="52">
+        <f t="shared" ref="M10:M18" si="4">F6</f>
+        <v>88.663980495747907</v>
+      </c>
+      <c r="N10" s="52">
+        <f t="shared" ref="N10:N18" si="5">K10</f>
+        <v>100.93831681151826</v>
+      </c>
+      <c r="O10" s="52">
+        <f t="shared" si="3"/>
+        <v>12.274336315770356</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>-209.57169473979818</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="1"/>
+        <v>-2272.0949726704434</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="K11" s="43">
+        <f t="shared" si="2"/>
+        <v>-41.318575995493134</v>
+      </c>
+      <c r="M11" s="52">
+        <f t="shared" si="4"/>
+        <v>-59.540729094989828</v>
+      </c>
+      <c r="N11" s="52">
+        <f t="shared" si="5"/>
+        <v>-41.318575995493134</v>
+      </c>
+      <c r="O11" s="52">
+        <f t="shared" si="3"/>
+        <v>18.222153099496694</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D12" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>-489.88432723500762</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>-3523.7509669819397</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="K12" s="43">
+        <f t="shared" si="2"/>
+        <v>-293.24654909859714</v>
+      </c>
+      <c r="M12" s="52">
+        <f t="shared" si="4"/>
+        <v>-319.0952997646279</v>
+      </c>
+      <c r="N12" s="52">
+        <f t="shared" si="5"/>
+        <v>-293.24654909859714</v>
+      </c>
+      <c r="O12" s="52">
+        <f t="shared" si="3"/>
+        <v>25.848750666030753</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D13" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>-914.3218881361862</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="1"/>
+        <v>-5183.4763036841832</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="K13" s="43">
+        <f t="shared" si="2"/>
+        <v>-700.6145711103004</v>
+      </c>
+      <c r="M13" s="52">
+        <f t="shared" si="4"/>
+        <v>-735.80493040668966</v>
+      </c>
+      <c r="N13" s="52">
+        <f t="shared" si="5"/>
+        <v>-700.6145711103004</v>
+      </c>
+      <c r="O13" s="52">
+        <f t="shared" si="3"/>
+        <v>35.190359296389261</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D14" s="40">
+        <v>2</v>
+      </c>
+      <c r="E14" s="41">
+        <f t="shared" si="0"/>
+        <v>-1526.5795879718441</v>
+      </c>
+      <c r="F14" s="41">
+        <f>((5*EXP(3*D12)*SIN(2*D12))-4*(5*EXP(3*D13)*SIN(2*D13))+3*(E14))/(2*C$4)</f>
+        <v>-7061.6776930289752</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="K14" s="43">
+        <f t="shared" si="2"/>
+        <v>-1319.4281482386803</v>
+      </c>
+      <c r="M14" s="52">
+        <f t="shared" si="4"/>
+        <v>-1365.4389310653848</v>
+      </c>
+      <c r="N14" s="52">
+        <f t="shared" si="5"/>
+        <v>-1319.4281482386803</v>
+      </c>
+      <c r="O14" s="52">
+        <f>ABS(M14-N14)</f>
+        <v>46.010782826704599</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="K15" s="43">
+        <f t="shared" si="2"/>
+        <v>-2214.4759194292033</v>
+      </c>
+      <c r="M15" s="52">
+        <f t="shared" si="4"/>
+        <v>-2272.0949726704434</v>
+      </c>
+      <c r="N15" s="52">
+        <f t="shared" si="5"/>
+        <v>-2214.4759194292033</v>
+      </c>
+      <c r="O15" s="52">
+        <f t="shared" si="3"/>
+        <v>57.619053241240181</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J16" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="K16" s="43">
+        <f t="shared" si="2"/>
+        <v>-3455.1336533198819</v>
+      </c>
+      <c r="M16" s="52">
+        <f t="shared" si="4"/>
+        <v>-3523.7509669819397</v>
+      </c>
+      <c r="N16" s="52">
+        <f t="shared" si="5"/>
+        <v>-3455.1336533198819</v>
+      </c>
+      <c r="O16" s="52">
+        <f t="shared" si="3"/>
+        <v>68.617313662057768</v>
+      </c>
+    </row>
+    <row r="17" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J17" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="K17" s="43">
+        <f t="shared" si="2"/>
+        <v>-5106.9103074957993</v>
+      </c>
+      <c r="M17" s="52">
+        <f t="shared" si="4"/>
+        <v>-5183.4763036841832</v>
+      </c>
+      <c r="N17" s="52">
+        <f t="shared" si="5"/>
+        <v>-5106.9103074957993</v>
+      </c>
+      <c r="O17" s="52">
+        <f t="shared" si="3"/>
+        <v>76.565996188383906</v>
+      </c>
+    </row>
+    <row r="18" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J18" s="40">
+        <v>2</v>
+      </c>
+      <c r="K18" s="43">
+        <f t="shared" si="2"/>
+        <v>-7216.7253373078292</v>
+      </c>
+      <c r="M18" s="52">
+        <f t="shared" si="4"/>
+        <v>-7061.6776930289752</v>
+      </c>
+      <c r="N18" s="52">
+        <f t="shared" si="5"/>
+        <v>-7216.7253373078292</v>
+      </c>
+      <c r="O18" s="52">
+        <f t="shared" si="3"/>
+        <v>155.04764427885402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF3B4F0-4A5F-4A3F-B2A5-F796568A93C4}">
+  <dimension ref="B1:N25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+    </row>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="46"/>
+    </row>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D12" s="51"/>
+      <c r="E12" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="51"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D15" s="30">
+        <v>1</v>
+      </c>
+      <c r="E15" s="31">
+        <f>5*EXP(3*D15)*SIN(2*D15)</f>
+        <v>91.318635203333841</v>
+      </c>
+      <c r="F15" s="31">
+        <f>(-25*(5*EXP(3*D15)*SIN(2*D15))+48*(5*EXP(3*D16)*SIN(2*D16))-36*(5*EXP(3*D17)*SIN(2*D17))+16*(5*EXP(3*D18)*SIN(2*D18))-3*(5*EXP(3*D19)*SIN(2*D19)))/(12*C$4)</f>
+        <v>192.07155592857109</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="43">
+        <f>5*(EXP(3*I15)*3*SIN(2*I15)+COS(2*I15)*2*EXP(3*I15))</f>
+        <v>190.37057910064783</v>
+      </c>
+      <c r="L15" s="52">
+        <f>F15</f>
+        <v>192.07155592857109</v>
+      </c>
+      <c r="M15" s="52">
+        <f>J15</f>
+        <v>190.37057910064783</v>
+      </c>
+      <c r="N15" s="52">
+        <f>ABS(L15-M15)</f>
+        <v>1.700976827923256</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E16" s="31">
+        <f t="shared" ref="E16:E25" si="0">5*EXP(3*D16)*SIN(2*D16)</f>
+        <v>109.60235532705481</v>
+      </c>
+      <c r="F16" s="31">
+        <f>(-25*(5*EXP(3*D16)*SIN(2*D16))+48*(5*EXP(3*D17)*SIN(2*D17))-36*(5*EXP(3*D18)*SIN(2*D18))+16*(5*EXP(3*D19)*SIN(2*D19))-3*(5*EXP(3*D20)*SIN(2*D20)))/(12*C$4)</f>
+        <v>171.20017226596408</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J16" s="43">
+        <f t="shared" ref="J16:J25" si="1">5*(EXP(3*I16)*3*SIN(2*I16)+COS(2*I16)*2*EXP(3*I16))</f>
+        <v>169.24888301568495</v>
+      </c>
+      <c r="L16" s="52">
+        <f>F16</f>
+        <v>171.20017226596408</v>
+      </c>
+      <c r="M16" s="52">
+        <f>J16</f>
+        <v>169.24888301568495</v>
+      </c>
+      <c r="N16" s="52">
+        <f>ABS(L16-M16)</f>
+        <v>1.9512892502791317</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D17" s="30">
+        <v>1.2</v>
+      </c>
+      <c r="E17" s="31">
+        <f t="shared" si="0"/>
+        <v>123.60379919941703</v>
+      </c>
+      <c r="F17" s="31">
+        <f>((5*EXP(3*D15)*SIN(2*D15))-8*(5*EXP(3*D16)*SIN(2*D16))+8*(5*EXP(3*D18)*SIN(2*D18))-(5*EXP(3*D19)*SIN(2*D19)))/(12*C$4)</f>
+        <v>101.23779218009288</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="J17" s="43">
+        <f t="shared" si="1"/>
+        <v>100.93831681151826</v>
+      </c>
+      <c r="L17" s="52">
+        <f t="shared" ref="L17:L25" si="2">F17</f>
+        <v>101.23779218009288</v>
+      </c>
+      <c r="M17" s="52">
+        <f t="shared" ref="M17:M25" si="3">J17</f>
+        <v>100.93831681151826</v>
+      </c>
+      <c r="N17" s="52">
+        <f t="shared" ref="N17:N25" si="4">ABS(L17-M17)</f>
+        <v>0.29947536857461898</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D18" s="30">
+        <v>1.3</v>
+      </c>
+      <c r="E18" s="31">
+        <f t="shared" si="0"/>
+        <v>127.33515142620439</v>
+      </c>
+      <c r="F18" s="31">
+        <f t="shared" ref="F18:F23" si="5">((5*EXP(3*D16)*SIN(2*D16))-8*(5*EXP(3*D17)*SIN(2*D17))+8*(5*EXP(3*D19)*SIN(2*D19))-(5*EXP(3*D20)*SIN(2*D20)))/(12*C$4)</f>
+        <v>-40.982418915173064</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="J18" s="43">
+        <f t="shared" si="1"/>
+        <v>-41.318575995493134</v>
+      </c>
+      <c r="L18" s="52">
+        <f t="shared" si="2"/>
+        <v>-40.982418915173064</v>
+      </c>
+      <c r="M18" s="52">
+        <f t="shared" si="3"/>
+        <v>-41.318575995493134</v>
+      </c>
+      <c r="N18" s="52">
+        <f t="shared" si="4"/>
+        <v>0.33615708032007063</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D19" s="30">
+        <v>1.4</v>
+      </c>
+      <c r="E19" s="31">
+        <f t="shared" si="0"/>
+        <v>111.69565338041906</v>
+      </c>
+      <c r="F19" s="31">
+        <f t="shared" si="5"/>
+        <v>-292.90278976922389</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="J19" s="43">
+        <f t="shared" si="1"/>
+        <v>-293.24654909859714</v>
+      </c>
+      <c r="L19" s="52">
+        <f t="shared" si="2"/>
+        <v>-292.90278976922389</v>
+      </c>
+      <c r="M19" s="52">
+        <f t="shared" si="3"/>
+        <v>-293.24654909859714</v>
+      </c>
+      <c r="N19" s="52">
+        <f t="shared" si="4"/>
+        <v>0.34375932937325615</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D20" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="E20" s="31">
+        <f t="shared" si="0"/>
+        <v>63.516091473278813</v>
+      </c>
+      <c r="F20" s="31">
+        <f t="shared" si="5"/>
+        <v>-700.3175354039173</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="J20" s="43">
+        <f t="shared" si="1"/>
+        <v>-700.6145711103004</v>
+      </c>
+      <c r="L20" s="52">
+        <f t="shared" si="2"/>
+        <v>-700.3175354039173</v>
+      </c>
+      <c r="M20" s="52">
+        <f t="shared" si="3"/>
+        <v>-700.6145711103004</v>
+      </c>
+      <c r="N20" s="52">
+        <f t="shared" si="4"/>
+        <v>0.29703570638309884</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D21" s="30">
+        <v>1.6</v>
+      </c>
+      <c r="E21" s="31">
+        <f t="shared" si="0"/>
+        <v>-35.465332700918879</v>
+      </c>
+      <c r="F21" s="31">
+        <f t="shared" si="5"/>
+        <v>-1319.2685909076572</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="J21" s="43">
+        <f t="shared" si="1"/>
+        <v>-1319.4281482386803</v>
+      </c>
+      <c r="L21" s="52">
+        <f t="shared" si="2"/>
+        <v>-1319.2685909076572</v>
+      </c>
+      <c r="M21" s="52">
+        <f t="shared" si="3"/>
+        <v>-1319.4281482386803</v>
+      </c>
+      <c r="N21" s="52">
+        <f t="shared" si="4"/>
+        <v>0.15955733102305203</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D22" s="30">
+        <v>1.7</v>
+      </c>
+      <c r="E22" s="31">
+        <f t="shared" si="0"/>
+        <v>-209.57169473979818</v>
+      </c>
+      <c r="F22" s="31">
+        <f t="shared" si="5"/>
+        <v>-2214.5949805527034</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="J22" s="43">
+        <f t="shared" si="1"/>
+        <v>-2214.4759194292033</v>
+      </c>
+      <c r="L22" s="52">
+        <f t="shared" si="2"/>
+        <v>-2214.5949805527034</v>
+      </c>
+      <c r="M22" s="52">
+        <f t="shared" si="3"/>
+        <v>-2214.4759194292033</v>
+      </c>
+      <c r="N22" s="52">
+        <f t="shared" si="4"/>
+        <v>0.11906112350015974</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D23" s="30">
+        <v>1.8</v>
+      </c>
+      <c r="E23" s="31">
+        <f t="shared" si="0"/>
+        <v>-489.88432723500762</v>
+      </c>
+      <c r="F23" s="31">
+        <f t="shared" si="5"/>
+        <v>-3455.739409916815</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="J23" s="43">
+        <f t="shared" si="1"/>
+        <v>-3455.1336533198819</v>
+      </c>
+      <c r="L23" s="52">
+        <f t="shared" si="2"/>
+        <v>-3455.739409916815</v>
+      </c>
+      <c r="M23" s="52">
+        <f t="shared" si="3"/>
+        <v>-3455.1336533198819</v>
+      </c>
+      <c r="N23" s="52">
+        <f t="shared" si="4"/>
+        <v>0.60575659693313355</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D24" s="30">
+        <v>1.9</v>
+      </c>
+      <c r="E24" s="31">
+        <f t="shared" si="0"/>
+        <v>-914.3218881361862</v>
+      </c>
+      <c r="F24" s="31">
+        <f>(3*(5*EXP(3*D20)*SIN(2*D20))-16*(5*EXP(3*D21)*SIN(2*D21))+36*(5*EXP(3*D22)*SIN(2*D22))-48*(5*EXP(3*D23)*SIN(2*D23))+25*(5*EXP(3*D24)*SIN(2*D24)))/(12*C$4)</f>
+        <v>-5108.4890909354053</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="J24" s="43">
+        <f t="shared" si="1"/>
+        <v>-5106.9103074957993</v>
+      </c>
+      <c r="L24" s="52">
+        <f t="shared" si="2"/>
+        <v>-5108.4890909354053</v>
+      </c>
+      <c r="M24" s="52">
+        <f t="shared" si="3"/>
+        <v>-5106.9103074957993</v>
+      </c>
+      <c r="N24" s="52">
+        <f t="shared" si="4"/>
+        <v>1.5787834396060134</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D25" s="48">
+        <v>2</v>
+      </c>
+      <c r="E25" s="49">
+        <f t="shared" si="0"/>
+        <v>-1526.5795879718441</v>
+      </c>
+      <c r="F25" s="49">
+        <f>(3*(5*EXP(3*D21)*SIN(2*D21))-16*(5*EXP(3*D22)*SIN(2*D22))+36*(5*EXP(3*D23)*SIN(2*D23))-48*(5*EXP(3*D24)*SIN(2*D24))+25*(5*EXP(3*D25)*SIN(2*D25)))/(12*C$4)</f>
+        <v>-7221.7697762378511</v>
+      </c>
+      <c r="G25" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="40">
+        <v>2</v>
+      </c>
+      <c r="J25" s="43">
+        <f t="shared" si="1"/>
+        <v>-7216.7253373078292</v>
+      </c>
+      <c r="L25" s="52">
+        <f t="shared" si="2"/>
+        <v>-7221.7697762378511</v>
+      </c>
+      <c r="M25" s="52">
+        <f t="shared" si="3"/>
+        <v>-7216.7253373078292</v>
+      </c>
+      <c r="N25" s="52">
+        <f t="shared" si="4"/>
+        <v>5.0444389300218972</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECE0C86-CE04-432A-9B60-B75C5A49672F}">
+  <dimension ref="C1:P54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1"/>
+      <c r="K2" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="61">
+        <f>COUNTA(F4:F20)</f>
+        <v>7</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F4" s="63">
+        <v>0</v>
+      </c>
+      <c r="G4" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="64">
+        <f>F4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="65">
+        <f>F4*G4</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F5" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="64">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="64">
+        <f t="shared" ref="H5:H13" si="0">F5*F5</f>
+        <v>0.25</v>
+      </c>
+      <c r="I5" s="65">
+        <f t="shared" ref="I5:I13" si="1">F5*G5</f>
+        <v>1.25</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F6" s="63">
+        <v>1</v>
+      </c>
+      <c r="G6" s="64">
+        <v>2</v>
+      </c>
+      <c r="H6" s="64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="65">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F7" s="63">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="64">
+        <v>4</v>
+      </c>
+      <c r="H7" s="64">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="I7" s="65">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="63">
+        <v>2</v>
+      </c>
+      <c r="G8" s="64">
+        <v>3.5</v>
+      </c>
+      <c r="H8" s="64">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="65">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F9" s="63">
+        <v>0</v>
+      </c>
+      <c r="G9" s="64">
+        <v>0</v>
+      </c>
+      <c r="H9" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="63">
+        <v>0</v>
+      </c>
+      <c r="G10" s="64">
+        <v>0</v>
+      </c>
+      <c r="H10" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="61">
+        <f>((K3*I21)-(F21*G21))/((K3*H21)-(F21*F21))</f>
+        <v>1.8636363636363635</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="61">
+        <f>(G21/K3)-K10*(F21/K3)</f>
+        <v>0.45454545454545459</v>
+      </c>
+      <c r="O10" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="P10" s="62"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="63"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="O11" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" s="62"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="63"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="68"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="70"/>
+      <c r="K14" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="18" t="str">
+        <f>"Y = "&amp;K10&amp;"x + "&amp;M10</f>
+        <v>Y = 1,86363636363636x + 0,454545454545455</v>
+      </c>
+      <c r="M14" s="72"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="19"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F15" s="68"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="73"/>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F16" s="68"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="70"/>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F17" s="68"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="74"/>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F18" s="68"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F19" s="68"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="70"/>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F20" s="68"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="70"/>
+      <c r="M20" s="75"/>
+    </row>
+    <row r="21" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="76">
+        <f>SUM(F4:F20)</f>
+        <v>5</v>
+      </c>
+      <c r="G21" s="77">
+        <f>SUM(G4:G20)</f>
+        <v>12.5</v>
+      </c>
+      <c r="H21" s="77">
+        <f>SUM(H4:H20)</f>
+        <v>7.5</v>
+      </c>
+      <c r="I21" s="78">
+        <f>SUM(I4:I20)</f>
+        <v>16.25</v>
+      </c>
+      <c r="K21" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="46"/>
+    </row>
+    <row r="33" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+    </row>
+    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+    </row>
+    <row r="41" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F41" s="51"/>
+      <c r="G41" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="51"/>
+    </row>
+    <row r="42" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="29"/>
+      <c r="K43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L43" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="N43" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="O43" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="P43" s="52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F44" s="30">
+        <v>0</v>
+      </c>
+      <c r="G44" s="31">
+        <f>1.8636*F44+0.4545</f>
+        <v>0.45450000000000002</v>
+      </c>
+      <c r="H44" s="31">
+        <f>(-25*(1.8636*F44+0.4545)+48*(1.8636*F45+0.4545)-36*(1.8636*F46+0.4545)+16*(1.8636*F47+0.4545)-3*(1.8636*F48+0.4545))/(12*E$33)</f>
+        <v>9.3179999999999872</v>
+      </c>
+      <c r="I44" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" s="5">
+        <v>1</v>
+      </c>
+      <c r="L44" s="43">
+        <f>5*(EXP(3*K44)*3*SIN(2*K44)+COS(2*K44)*2*EXP(3*K44))</f>
+        <v>190.37057910064783</v>
+      </c>
+      <c r="N44" s="52">
+        <f>H44</f>
+        <v>9.3179999999999872</v>
+      </c>
+      <c r="O44" s="52">
+        <f>L44</f>
+        <v>190.37057910064783</v>
+      </c>
+      <c r="P44" s="52">
+        <f>ABS(N44-O44)</f>
+        <v>181.05257910064785</v>
+      </c>
+    </row>
+    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G45" s="31">
+        <f t="shared" ref="G45:H54" si="2">5*EXP(3*F45)*SIN(2*F45)</f>
+        <v>18.856056578100787</v>
+      </c>
+      <c r="H45" s="31">
+        <f>(-25*(1.8636*F45+0.4545)+48*(1.8636*F46+0.4545)-36*(1.8636*F47+0.4545)+16*(1.8636*F48+0.4545)-3*(1.8636*F49+0.4545))/(12*E$33)</f>
+        <v>20.965500000000002</v>
+      </c>
+      <c r="I45" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L45" s="43">
+        <f t="shared" ref="L45:L54" si="3">5*(EXP(3*K45)*3*SIN(2*K45)+COS(2*K45)*2*EXP(3*K45))</f>
+        <v>169.24888301568495</v>
+      </c>
+      <c r="N45" s="52">
+        <f>H45</f>
+        <v>20.965500000000002</v>
+      </c>
+      <c r="O45" s="52">
+        <f>L45</f>
+        <v>169.24888301568495</v>
+      </c>
+      <c r="P45" s="52">
+        <f>ABS(N45-O45)</f>
+        <v>148.28338301568496</v>
+      </c>
+    </row>
+    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F46" s="30">
+        <v>1</v>
+      </c>
+      <c r="G46" s="31">
+        <f t="shared" si="2"/>
+        <v>91.318635203333841</v>
+      </c>
+      <c r="H46" s="31">
+        <f>(1.3686*F44+0.4545)-8*(1.8636*F45+0.4545)+8*(1.3686*F47+0.4545)-(1.3686*F48+0.4545)/(12*E$33)</f>
+        <v>6.7635500000000022</v>
+      </c>
+      <c r="I46" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K46" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="L46" s="43">
+        <f t="shared" si="3"/>
+        <v>100.93831681151826</v>
+      </c>
+      <c r="N46" s="52">
+        <f t="shared" ref="N46:N54" si="4">H46</f>
+        <v>6.7635500000000022</v>
+      </c>
+      <c r="O46" s="52">
+        <f t="shared" ref="O46:O54" si="5">L46</f>
+        <v>100.93831681151826</v>
+      </c>
+      <c r="P46" s="52">
+        <f t="shared" ref="P46:P54" si="6">ABS(N46-O46)</f>
+        <v>94.174766811518253</v>
+      </c>
+    </row>
+    <row r="47" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F47" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="G47" s="49">
+        <f t="shared" si="2"/>
+        <v>63.516091473278813</v>
+      </c>
+      <c r="H47" s="31">
+        <f>(1.3686*F45+0.4545)-8*(1.8636*F46+0.4545)+8*(1.3686*F48+0.4545)-(1.3686*F49+0.4545)/(12*E$33)</f>
+        <v>7.7488500000000009</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K47" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="L47" s="43">
+        <f t="shared" si="3"/>
+        <v>-41.318575995493134</v>
+      </c>
+      <c r="N47" s="52">
+        <f t="shared" si="4"/>
+        <v>7.7488500000000009</v>
+      </c>
+      <c r="O47" s="52">
+        <f t="shared" si="5"/>
+        <v>-41.318575995493134</v>
+      </c>
+      <c r="P47" s="52">
+        <f t="shared" si="6"/>
+        <v>49.067425995493139</v>
+      </c>
+    </row>
+    <row r="48" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F48" s="30">
+        <v>2</v>
+      </c>
+      <c r="G48" s="79">
+        <f t="shared" si="2"/>
+        <v>-1526.5795879718441</v>
+      </c>
+      <c r="H48" s="49">
+        <f>(3*(1.3686*F44+0.4545)-16*(1.3686*F45+0.4545)+36*(1.3686*F46+0.4545)-48*(1.8636*F47-0.4545)+25*(1.3686*F48+0.4545))/(12*E$33)</f>
+        <v>13.503</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="L48" s="43">
+        <f t="shared" si="3"/>
+        <v>-293.24654909859714</v>
+      </c>
+      <c r="N48" s="52">
+        <f t="shared" si="4"/>
+        <v>13.503</v>
+      </c>
+      <c r="O48" s="52">
+        <f t="shared" si="5"/>
+        <v>-293.24654909859714</v>
+      </c>
+      <c r="P48" s="52">
+        <f t="shared" si="6"/>
+        <v>306.74954909859713</v>
+      </c>
+    </row>
+    <row r="49" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
+      <c r="K49" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="L49" s="43">
+        <f t="shared" si="3"/>
+        <v>-700.6145711103004</v>
+      </c>
+      <c r="N49" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="52">
+        <f t="shared" si="5"/>
+        <v>-700.6145711103004</v>
+      </c>
+      <c r="P49" s="52">
+        <f t="shared" si="6"/>
+        <v>700.6145711103004</v>
+      </c>
+    </row>
+    <row r="50" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="K50" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="L50" s="43">
+        <f t="shared" si="3"/>
+        <v>-1319.4281482386803</v>
+      </c>
+      <c r="N50" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="52">
+        <f t="shared" si="5"/>
+        <v>-1319.4281482386803</v>
+      </c>
+      <c r="P50" s="52">
+        <f t="shared" si="6"/>
+        <v>1319.4281482386803</v>
+      </c>
+    </row>
+    <row r="51" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="K51" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="L51" s="43">
+        <f t="shared" si="3"/>
+        <v>-2214.4759194292033</v>
+      </c>
+      <c r="N51" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O51" s="52">
+        <f t="shared" si="5"/>
+        <v>-2214.4759194292033</v>
+      </c>
+      <c r="P51" s="52">
+        <f t="shared" si="6"/>
+        <v>2214.4759194292033</v>
+      </c>
+    </row>
+    <row r="52" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
+      <c r="K52" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="L52" s="43">
+        <f t="shared" si="3"/>
+        <v>-3455.1336533198819</v>
+      </c>
+      <c r="N52" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O52" s="52">
+        <f t="shared" si="5"/>
+        <v>-3455.1336533198819</v>
+      </c>
+      <c r="P52" s="52">
+        <f t="shared" si="6"/>
+        <v>3455.1336533198819</v>
+      </c>
+    </row>
+    <row r="53" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="K53" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="L53" s="43">
+        <f t="shared" si="3"/>
+        <v>-5106.9103074957993</v>
+      </c>
+      <c r="N53" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O53" s="52">
+        <f t="shared" si="5"/>
+        <v>-5106.9103074957993</v>
+      </c>
+      <c r="P53" s="52">
+        <f t="shared" si="6"/>
+        <v>5106.9103074957993</v>
+      </c>
+    </row>
+    <row r="54" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="K54" s="40">
+        <v>2</v>
+      </c>
+      <c r="L54" s="43">
+        <f t="shared" si="3"/>
+        <v>-7216.7253373078292</v>
+      </c>
+      <c r="N54" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O54" s="52">
+        <f t="shared" si="5"/>
+        <v>-7216.7253373078292</v>
+      </c>
+      <c r="P54" s="52">
+        <f t="shared" si="6"/>
+        <v>7216.7253373078292</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>